<commit_message>
feat: add API endpoint and weather API's integration
For Project 03: Add API endpoint, integrate OpenWeatherMap API and fetch data from the app endpoint.
</commit_message>
<xml_diff>
--- a/3- Web APIs and Asynchronous/Project_03_Rubric.xlsx
+++ b/3- Web APIs and Asynchronous/Project_03_Rubric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danihergar/Documents/Repositories/udacity_Front_End_Web_Developer/3- Web APIs and Asynchronous/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D249E9A1-65D2-9D48-91CC-3273E9D478AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3B051F-A56F-7446-BBCD-F8A372CC1809}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="16000" xr2:uid="{DB850500-CB71-2948-A340-54DF47885E39}"/>
   </bookViews>
@@ -731,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9D9673A-9885-9E49-AA6A-68581B46E0B8}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -772,18 +772,18 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="18">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -802,18 +802,18 @@
       </c>
     </row>
     <row r="12" spans="1:2" ht="19">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="95">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -826,10 +826,10 @@
       </c>
     </row>
     <row r="15" spans="1:2" ht="57">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="5" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: add POST/GET routes and update UI functionality
</commit_message>
<xml_diff>
--- a/3- Web APIs and Asynchronous/Project_03_Rubric.xlsx
+++ b/3- Web APIs and Asynchronous/Project_03_Rubric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danihergar/Documents/Repositories/udacity_Front_End_Web_Developer/3- Web APIs and Asynchronous/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3B051F-A56F-7446-BBCD-F8A372CC1809}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB8EC86-9AF6-C74D-9628-A34965AFE599}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="16000" xr2:uid="{DB850500-CB71-2948-A340-54DF47885E39}"/>
   </bookViews>
@@ -392,16 +392,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -731,21 +725,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9D9673A-9885-9E49-AA6A-68581B46E0B8}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="50.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="147.5" style="4" customWidth="1"/>
+    <col min="1" max="1" width="50.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="147.5" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="20">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
+      <c r="B1" s="5"/>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
@@ -756,42 +750,42 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="76">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="76">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="20">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="7"/>
+      <c r="B9" s="5"/>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
@@ -802,50 +796,50 @@
       </c>
     </row>
     <row r="12" spans="1:2" ht="19">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="95">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="57">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="57">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="133">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="20">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="7"/>
+      <c r="B18" s="5"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
@@ -856,34 +850,34 @@
       </c>
     </row>
     <row r="21" spans="1:2" ht="114">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="95">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="76">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="76">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="4" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: add package.json for dependencies
</commit_message>
<xml_diff>
--- a/3- Web APIs and Asynchronous/Project_03_Rubric.xlsx
+++ b/3- Web APIs and Asynchronous/Project_03_Rubric.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danihergar/Documents/Repositories/udacity_Front_End_Web_Developer/3- Web APIs and Asynchronous/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB8EC86-9AF6-C74D-9628-A34965AFE599}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B058BBE7-221E-A64E-9972-8E335B367670}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="460" windowWidth="28040" windowHeight="16000" xr2:uid="{DB850500-CB71-2948-A340-54DF47885E39}"/>
   </bookViews>
@@ -725,7 +725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9D9673A-9885-9E49-AA6A-68581B46E0B8}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>

</xml_diff>